<commit_message>
update timesheet period july
</commit_message>
<xml_diff>
--- a/8_Period_20_Jul_2024_sd_19_Aug_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Juli.xlsx
+++ b/8_Period_20_Jul_2024_sd_19_Aug_2024/Timesheet Danamon-Bayu Bagus Bagaswara-Juli.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\timesheet-danamon\8_Period_20_Jul_2024_sd_19_Aug_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\8_Period_20_Jul_2024_sd_19_Aug_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F576B-2400-4FB0-B634-F58991652BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E2B535-FFA5-4FE6-99F9-3BDCBFA9AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>TIME SHEET</t>
   </si>
@@ -175,16 +175,19 @@
     <t>Bayu Bagus Bagaswara</t>
   </si>
   <si>
-    <t>Diskusi alur bisnis Billing dengan User</t>
-  </si>
-  <si>
-    <t>Pengembangan fitur Billing</t>
-  </si>
-  <si>
-    <t>Diskusi dengan tim developer Billing</t>
-  </si>
-  <si>
     <t>20 Juli - 19 Agustus</t>
+  </si>
+  <si>
+    <t>Preparation implementation Release 8 - Billing</t>
+  </si>
+  <si>
+    <t>Discuss Release 9B - Regulatory (LKPBU &amp; LBABK)</t>
+  </si>
+  <si>
+    <t>Development Release 9B - Regulatory (LKPBU &amp; LBABK)</t>
+  </si>
+  <si>
+    <t>PAT Release 8</t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -656,6 +659,9 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -698,20 +704,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1102,7 +1102,7 @@
   <dimension ref="A1:EQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -1198,10 +1198,10 @@
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="66" t="s">
+      <c r="S5" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="67"/>
+      <c r="T5" s="68"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10" t="s">
         <v>24</v>
@@ -1228,43 +1228,43 @@
       <c r="B6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="71">
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="72">
         <v>2024</v>
       </c>
-      <c r="T6" s="72"/>
-      <c r="U6" s="71" t="s">
+      <c r="T6" s="73"/>
+      <c r="U6" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="72"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="66"/>
+      <c r="Z6" s="73"/>
       <c r="AA6" s="23"/>
-      <c r="AB6" s="65"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="65"/>
-      <c r="AE6" s="65"/>
+      <c r="AB6" s="66"/>
+      <c r="AC6" s="66"/>
+      <c r="AD6" s="66"/>
+      <c r="AE6" s="66"/>
       <c r="AF6" s="57"/>
       <c r="AG6" s="57"/>
       <c r="AH6" s="56"/>
@@ -1526,10 +1526,10 @@
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="53"/>
-      <c r="E10" s="73">
-        <v>1</v>
-      </c>
-      <c r="F10" s="73">
+      <c r="E10" s="49">
+        <v>1</v>
+      </c>
+      <c r="F10" s="49">
         <v>1</v>
       </c>
       <c r="G10" s="49">
@@ -1541,12 +1541,14 @@
       <c r="I10" s="58">
         <v>1</v>
       </c>
-      <c r="J10" s="53"/>
+      <c r="J10" s="74" t="s">
+        <v>31</v>
+      </c>
       <c r="K10" s="53"/>
-      <c r="L10" s="73">
-        <v>1</v>
-      </c>
-      <c r="M10" s="73">
+      <c r="L10" s="49">
+        <v>1</v>
+      </c>
+      <c r="M10" s="49">
         <v>1</v>
       </c>
       <c r="N10" s="49">
@@ -1560,10 +1562,10 @@
       </c>
       <c r="Q10" s="53"/>
       <c r="R10" s="53"/>
-      <c r="S10" s="73">
-        <v>1</v>
-      </c>
-      <c r="T10" s="73">
+      <c r="S10" s="49">
+        <v>1</v>
+      </c>
+      <c r="T10" s="49">
         <v>1</v>
       </c>
       <c r="U10" s="49">
@@ -1577,10 +1579,10 @@
       </c>
       <c r="X10" s="53"/>
       <c r="Y10" s="53"/>
-      <c r="Z10" s="73">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="73">
+      <c r="Z10" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="49">
         <v>1</v>
       </c>
       <c r="AB10" s="49">
@@ -1601,10 +1603,10 @@
         <f>SUM(C10:AG10)</f>
         <v>21</v>
       </c>
-      <c r="AI10" s="59" t="s">
+      <c r="AI10" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="AJ10" s="61"/>
+      <c r="AJ10" s="62"/>
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
       <c r="AM10" s="6"/>
@@ -1720,33 +1722,37 @@
     <row r="11" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A11" s="36"/>
       <c r="B11" s="47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="74"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="50"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="54"/>
+      <c r="H11" s="44">
+        <v>5</v>
+      </c>
+      <c r="I11" s="44">
+        <v>5</v>
+      </c>
+      <c r="J11" s="75"/>
       <c r="K11" s="54"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
       <c r="N11" s="50"/>
       <c r="O11" s="50"/>
       <c r="P11" s="50"/>
       <c r="Q11" s="54"/>
       <c r="R11" s="54"/>
-      <c r="S11" s="74"/>
-      <c r="T11" s="74"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
       <c r="U11" s="50"/>
       <c r="V11" s="50"/>
       <c r="W11" s="50"/>
       <c r="X11" s="54"/>
       <c r="Y11" s="54"/>
-      <c r="Z11" s="74"/>
-      <c r="AA11" s="74"/>
+      <c r="Z11" s="50"/>
+      <c r="AA11" s="50"/>
       <c r="AB11" s="50"/>
       <c r="AC11" s="50"/>
       <c r="AD11" s="50"/>
@@ -1755,41 +1761,47 @@
       <c r="AG11" s="50"/>
       <c r="AH11" s="44">
         <f>SUM(C11:AG11)</f>
-        <v>0</v>
-      </c>
-      <c r="AI11" s="60"/>
-      <c r="AJ11" s="62"/>
+        <v>10</v>
+      </c>
+      <c r="AI11" s="61"/>
+      <c r="AJ11" s="63"/>
     </row>
     <row r="12" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A12" s="36"/>
       <c r="B12" s="47" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="50"/>
+      <c r="E12" s="59">
+        <v>4</v>
+      </c>
+      <c r="F12" s="50">
+        <v>4</v>
+      </c>
+      <c r="G12" s="50">
+        <v>7</v>
+      </c>
       <c r="H12" s="44"/>
       <c r="I12" s="44"/>
-      <c r="J12" s="54"/>
+      <c r="J12" s="75"/>
       <c r="K12" s="54"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
       <c r="N12" s="50"/>
       <c r="O12" s="50"/>
       <c r="P12" s="50"/>
       <c r="Q12" s="54"/>
       <c r="R12" s="54"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
       <c r="U12" s="50"/>
       <c r="V12" s="50"/>
       <c r="W12" s="50"/>
       <c r="X12" s="54"/>
       <c r="Y12" s="54"/>
-      <c r="Z12" s="74"/>
-      <c r="AA12" s="74"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
       <c r="AB12" s="50"/>
       <c r="AC12" s="50"/>
       <c r="AD12" s="50"/>
@@ -1798,41 +1810,49 @@
       <c r="AG12" s="50"/>
       <c r="AH12" s="44">
         <f>SUM(C12:AG12)</f>
-        <v>0</v>
-      </c>
-      <c r="AI12" s="60"/>
-      <c r="AJ12" s="62"/>
+        <v>15</v>
+      </c>
+      <c r="AI12" s="61"/>
+      <c r="AJ12" s="63"/>
     </row>
     <row r="13" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A13" s="36"/>
       <c r="B13" s="47" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="74"/>
+      <c r="E13" s="59">
+        <v>3</v>
+      </c>
+      <c r="F13" s="50">
+        <v>3</v>
+      </c>
       <c r="G13" s="50"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="54"/>
+      <c r="H13" s="44">
+        <v>1</v>
+      </c>
+      <c r="I13" s="44">
+        <v>1</v>
+      </c>
+      <c r="J13" s="76"/>
       <c r="K13" s="54"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
       <c r="N13" s="50"/>
       <c r="O13" s="50"/>
       <c r="P13" s="50"/>
       <c r="Q13" s="54"/>
       <c r="R13" s="54"/>
-      <c r="S13" s="74"/>
-      <c r="T13" s="74"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
       <c r="U13" s="50"/>
       <c r="V13" s="50"/>
       <c r="W13" s="50"/>
       <c r="X13" s="54"/>
       <c r="Y13" s="54"/>
-      <c r="Z13" s="74"/>
-      <c r="AA13" s="74"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
       <c r="AB13" s="50"/>
       <c r="AC13" s="50"/>
       <c r="AD13" s="50"/>
@@ -1841,10 +1861,10 @@
       <c r="AG13" s="50"/>
       <c r="AH13" s="44">
         <f>SUM(C13:AG13)</f>
-        <v>0</v>
-      </c>
-      <c r="AI13" s="60"/>
-      <c r="AJ13" s="62"/>
+        <v>8</v>
+      </c>
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="63"/>
     </row>
     <row r="14" spans="1:147" s="4" customFormat="1" ht="36" customHeight="1">
       <c r="A14" s="37" t="s">
@@ -1859,39 +1879,39 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="75">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F14" s="75">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="E14" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="G14" s="51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H14" s="45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I14" s="45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J14" s="55">
-        <f t="shared" si="0"/>
+        <f>SUM(J10:J13)</f>
         <v>0</v>
       </c>
       <c r="K14" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="75">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M14" s="75">
+      <c r="L14" s="51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="51">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1915,11 +1935,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S14" s="75">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T14" s="75">
+      <c r="S14" s="51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="T14" s="51">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1943,11 +1963,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="75">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AA14" s="75">
+      <c r="Z14" s="51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA14" s="51">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1977,7 +1997,7 @@
       </c>
       <c r="AH14" s="45">
         <f>SUM(C14:AG14)</f>
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="AI14" s="39"/>
       <c r="AJ14" s="40"/>
@@ -2033,7 +2053,7 @@
       <c r="Z19" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="AI10:AI13"/>
     <mergeCell ref="AJ10:AJ13"/>
     <mergeCell ref="C6:N6"/>
@@ -2042,6 +2062,7 @@
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:Z6"/>
+    <mergeCell ref="J10:J13"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.19" header="0.5" footer="0.16"/>

</xml_diff>